<commit_message>
add BBC health check to press site
</commit_message>
<xml_diff>
--- a/data/press.xlsx
+++ b/data/press.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/layalliverpool/Documents/WEBSITE/layallivs.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AA62C5-4CF1-2249-9E11-F4BC90B3B91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC25681-90F1-8448-9736-3A6D06EA1152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28540" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WEBSITE" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="243">
   <si>
     <t>Outlet</t>
   </si>
@@ -1129,6 +1129,30 @@
   <si>
     <t>https://open.spotify.com/episode/5C4D0AJksdPGBOLmQp55xl?si=-dkgb8ozSCKUkHYrUcgRRQ</t>
   </si>
+  <si>
+    <t>https://www.amnesty.de/informieren/amnesty-journal/rassismus-im-gesundheitssystem-buch-racism-kills-layal-liverpool-diagnose-unsichtbar</t>
+  </si>
+  <si>
+    <t>Diagnosis: Invisible</t>
+  </si>
+  <si>
+    <t>Amnesty Journal</t>
+  </si>
+  <si>
+    <t>Interview: Making human blood deadly to mosquitoes — 30 July 2025</t>
+  </si>
+  <si>
+    <t>Interview: What surpassing 1.5°C means for global health — 29 October 2025</t>
+  </si>
+  <si>
+    <t>https://www.bbc.co.uk/programmes/w3ct6vjm</t>
+  </si>
+  <si>
+    <t>https://www.bbc.co.uk/programmes/w3ct6vk6</t>
+  </si>
+  <si>
+    <t>Interview: What surpassing 1.5°C means for global health</t>
+  </si>
 </sst>
 </file>
 
@@ -1137,7 +1161,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1219,8 +1243,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1237,6 +1273,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9F2D0"/>
         <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1271,10 +1313,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1336,8 +1379,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1551,10 +1607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1612,16 +1668,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>242</v>
       </c>
       <c r="C2" s="4">
-        <v>45665</v>
+        <v>45959</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
+      <c r="E2" s="28" t="s">
+        <v>241</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1647,20 +1703,20 @@
       <c r="AA2" s="2"/>
     </row>
     <row r="3" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>9</v>
+      <c r="A3" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>238</v>
       </c>
       <c r="C3" s="4">
-        <v>45600</v>
+        <v>45868</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
+      <c r="E3" s="28" t="s">
+        <v>240</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1686,20 +1742,20 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>13</v>
+      <c r="A4" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4">
-        <v>45589</v>
+        <v>45665</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1725,20 +1781,20 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
+      <c r="A5" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4">
-        <v>45583</v>
+        <v>45600</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1764,20 +1820,20 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
+      <c r="A6" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4">
-        <v>45498</v>
+        <v>45589</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1804,19 +1860,19 @@
     </row>
     <row r="7" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4">
-        <v>45497</v>
+        <v>45583</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1843,19 +1899,19 @@
     </row>
     <row r="8" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4">
-        <v>45492</v>
+        <v>45498</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="2"/>
@@ -1882,19 +1938,19 @@
     </row>
     <row r="9" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4">
-        <v>45489</v>
+        <v>45497</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="2"/>
@@ -1921,19 +1977,19 @@
     </row>
     <row r="10" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C10" s="4">
-        <v>45484</v>
+        <v>45492</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="2"/>
@@ -1960,19 +2016,19 @@
     </row>
     <row r="11" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C11" s="4">
-        <v>45481</v>
+        <v>45489</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>234</v>
+        <v>32</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="2"/>
@@ -1998,20 +2054,20 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>39</v>
+      <c r="A12" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4">
-        <v>45475</v>
+        <v>45484</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="2"/>
@@ -2038,19 +2094,19 @@
     </row>
     <row r="13" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4">
-        <v>45470</v>
+        <v>45481</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>44</v>
+        <v>234</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="2"/>
@@ -2076,20 +2132,20 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>33</v>
+      <c r="A14" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C14" s="4">
-        <v>45463</v>
+        <v>45475</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="2"/>
@@ -2116,17 +2172,19 @@
     </row>
     <row r="15" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C15" s="4">
-        <v>45460</v>
+        <v>45470</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="E15" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="2"/>
@@ -2153,19 +2211,19 @@
     </row>
     <row r="16" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C16" s="4">
-        <v>45461</v>
+        <v>45463</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="2"/>
@@ -2191,20 +2249,18 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>53</v>
+      <c r="A17" s="3" t="s">
+        <v>47</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>54</v>
+      <c r="B17" s="3" t="s">
+        <v>48</v>
       </c>
-      <c r="C17" s="10">
-        <v>45453</v>
+      <c r="C17" s="4">
+        <v>45460</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>55</v>
+      <c r="D17" s="3"/>
+      <c r="E17" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="2"/>
@@ -2230,20 +2286,20 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>56</v>
+      <c r="A18" s="3" t="s">
+        <v>50</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>57</v>
+      <c r="B18" s="3" t="s">
+        <v>51</v>
       </c>
-      <c r="C18" s="10">
-        <v>45451</v>
+      <c r="C18" s="4">
+        <v>45461</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>58</v>
+      <c r="E18" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="2"/>
@@ -2270,19 +2326,19 @@
     </row>
     <row r="19" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C19" s="10">
-        <v>45449</v>
+        <v>45453</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="2"/>
@@ -2308,20 +2364,20 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>62</v>
+      <c r="A20" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C20" s="10">
-        <v>45448</v>
+        <v>45451</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>64</v>
+      <c r="E20" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="2"/>
@@ -2347,20 +2403,20 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>65</v>
+      <c r="A21" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C21" s="10">
-        <v>45441</v>
+        <v>45449</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="2"/>
@@ -2387,19 +2443,19 @@
     </row>
     <row r="22" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C22" s="10">
-        <v>45437</v>
+        <v>45448</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>71</v>
+      <c r="E22" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="2"/>
@@ -2426,19 +2482,19 @@
     </row>
     <row r="23" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C23" s="10">
-        <v>45437</v>
+        <v>45441</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="2"/>
@@ -2465,19 +2521,19 @@
     </row>
     <row r="24" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C24" s="10">
-        <v>45387</v>
+        <v>45437</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="2"/>
@@ -2504,19 +2560,19 @@
     </row>
     <row r="25" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C25" s="10">
-        <v>44392</v>
+        <v>45437</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="2"/>
@@ -2542,20 +2598,20 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
-        <v>81</v>
+      <c r="A26" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C26" s="10">
-        <v>43963</v>
+        <v>45387</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="2"/>
@@ -2582,19 +2638,19 @@
     </row>
     <row r="27" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C27" s="10">
-        <v>43882</v>
+        <v>44392</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="2"/>
@@ -2620,11 +2676,21 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="A28" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="10">
+        <v>43963</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="F28" s="7"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -2649,11 +2715,21 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="A29" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="10">
+        <v>43882</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -2707,11 +2783,11 @@
       <c r="AA30" s="2"/>
     </row>
     <row r="31" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
       <c r="F31" s="7"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -2736,11 +2812,11 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
       <c r="F32" s="7"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -30836,33 +30912,49 @@
       <c r="Z1000" s="2"/>
       <c r="AA1000" s="2"/>
     </row>
+    <row r="1001" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1001" s="14"/>
+      <c r="B1001" s="14"/>
+      <c r="C1001" s="14"/>
+      <c r="D1001" s="14"/>
+      <c r="E1001" s="14"/>
+    </row>
+    <row r="1002" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1002" s="14"/>
+      <c r="B1002" s="14"/>
+      <c r="C1002" s="14"/>
+      <c r="D1002" s="14"/>
+      <c r="E1002" s="14"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="E25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E3" r:id="rId26" xr:uid="{12BF1512-FED2-A842-9F95-73FD58DD0DF1}"/>
+    <hyperlink ref="E2" r:id="rId27" xr:uid="{16ACB4A7-641F-1C49-BAA7-4D0AF71FAA45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -30871,14 +30963,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="2" max="2" width="91.33203125" style="27" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="48.1640625" customWidth="1"/>
     <col min="5" max="5" width="49.33203125" customWidth="1"/>
@@ -31080,13 +31174,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>101</v>
+        <v>239</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
+      <c r="D6" s="26" t="s">
+        <v>241</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>102</v>
@@ -31114,19 +31208,21 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>103</v>
+      <c r="A7" s="3" t="s">
+        <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>104</v>
+      <c r="B7" s="3" t="s">
+        <v>238</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>11</v>
+      <c r="C7" s="25" t="s">
+        <v>7</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>105</v>
+      <c r="D7" s="26" t="s">
+        <v>240</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -31150,20 +31246,20 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>106</v>
+      <c r="A8" s="25" t="s">
+        <v>237</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>107</v>
+      <c r="B8" s="25" t="s">
+        <v>236</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>108</v>
+      <c r="D8" s="26" t="s">
+        <v>235</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="7"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -31186,22 +31282,22 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>9</v>
+      <c r="A9" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -31224,22 +31320,20 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>13</v>
+      <c r="A10" s="16" t="s">
+        <v>103</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>111</v>
+      <c r="B10" s="13" t="s">
+        <v>104</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>15</v>
+      <c r="D10" s="17" t="s">
+        <v>105</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F10" s="7"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -31263,16 +31357,16 @@
     </row>
     <row r="11" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="7"/>
@@ -31298,20 +31392,20 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
+      <c r="A12" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>117</v>
+      <c r="E12" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="2"/>
@@ -31336,19 +31430,21 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>118</v>
+      <c r="A13" s="6" t="s">
+        <v>13</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>119</v>
+      <c r="B13" s="3" t="s">
+        <v>111</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>120</v>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>121</v>
+      <c r="D13" s="5" t="s">
+        <v>15</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -31372,17 +31468,19 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
-        <v>122</v>
+      <c r="A14" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18" t="s">
-        <v>124</v>
+      <c r="C14" s="13" t="s">
+        <v>11</v>
       </c>
+      <c r="D14" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="13"/>
       <c r="F14" s="7"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -31406,20 +31504,20 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>125</v>
+      <c r="A15" s="3" t="s">
+        <v>16</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>126</v>
+      <c r="B15" s="3" t="s">
+        <v>116</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>7</v>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>127</v>
+      <c r="D15" s="5" t="s">
+        <v>19</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>128</v>
+      <c r="E15" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="2"/>
@@ -31444,14 +31542,18 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>129</v>
+      <c r="A16" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>121</v>
+      </c>
       <c r="E16" s="13"/>
       <c r="F16" s="7"/>
       <c r="G16" s="2"/>
@@ -31476,19 +31578,17 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>131</v>
+      <c r="A17" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>11</v>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="18" t="s">
+        <v>124</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="E17" s="13"/>
       <c r="F17" s="7"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -31513,15 +31613,19 @@
     </row>
     <row r="18" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>127</v>
+      </c>
       <c r="E18" s="13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="2"/>
@@ -31546,21 +31650,15 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>137</v>
+      <c r="A19" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>140</v>
-      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
       <c r="F19" s="7"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -31584,21 +31682,19 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>20</v>
+      <c r="A20" s="16" t="s">
+        <v>131</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>141</v>
+      <c r="B20" s="13" t="s">
+        <v>132</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>7</v>
+      <c r="C20" s="13" t="s">
+        <v>11</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>22</v>
+      <c r="D20" s="18" t="s">
+        <v>133</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="E20" s="13"/>
       <c r="F20" s="7"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -31622,20 +31718,16 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>5</v>
+      <c r="A21" s="13" t="s">
+        <v>134</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>143</v>
+      <c r="B21" s="13" t="s">
+        <v>135</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>102</v>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="2"/>
@@ -31660,20 +31752,20 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>25</v>
+      <c r="A22" s="16" t="s">
+        <v>137</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>144</v>
+      <c r="B22" s="13" t="s">
+        <v>138</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
+      <c r="C22" s="13" t="s">
+        <v>120</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>28</v>
+      <c r="D22" s="18" t="s">
+        <v>139</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>145</v>
+      <c r="E22" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="2"/>
@@ -31698,19 +31790,21 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>146</v>
+      <c r="A23" s="3" t="s">
+        <v>20</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>147</v>
+      <c r="B23" s="3" t="s">
+        <v>141</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>11</v>
+      <c r="C23" s="3" t="s">
+        <v>7</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>148</v>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
       </c>
-      <c r="E23" s="19"/>
+      <c r="E23" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="F23" s="7"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -31735,18 +31829,20 @@
     </row>
     <row r="24" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
-      <c r="E24" s="20"/>
+      <c r="E24" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -31771,18 +31867,20 @@
     </row>
     <row r="25" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
-      <c r="E25" s="20"/>
+      <c r="E25" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="F25" s="7"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -31806,21 +31904,19 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>36</v>
+      <c r="A26" s="16" t="s">
+        <v>146</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>151</v>
+      <c r="B26" s="13" t="s">
+        <v>147</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>7</v>
+      <c r="C26" s="13" t="s">
+        <v>11</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>38</v>
+      <c r="D26" s="18" t="s">
+        <v>148</v>
       </c>
-      <c r="E26" s="20" t="s">
-        <v>152</v>
-      </c>
+      <c r="E26" s="19"/>
       <c r="F26" s="7"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -31844,15 +31940,19 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
-        <v>153</v>
+      <c r="A27" s="3" t="s">
+        <v>29</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>154</v>
+      <c r="B27" s="3" t="s">
+        <v>149</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="21"/>
+      <c r="C27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="20"/>
       <c r="F27" s="7"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -31876,21 +31976,19 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>39</v>
+      <c r="A28" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>156</v>
-      </c>
+      <c r="E28" s="20"/>
       <c r="F28" s="7"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -31915,18 +32013,20 @@
     </row>
     <row r="29" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
-      <c r="E29" s="20"/>
+      <c r="E29" s="20" t="s">
+        <v>152</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -31951,17 +32051,13 @@
     </row>
     <row r="30" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>160</v>
-      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
       <c r="E30" s="21"/>
       <c r="F30" s="7"/>
       <c r="G30" s="2"/>
@@ -31986,19 +32082,21 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>33</v>
+      <c r="A31" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
-      <c r="E31" s="20"/>
+      <c r="E31" s="20" t="s">
+        <v>156</v>
+      </c>
       <c r="F31" s="7"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -32023,18 +32121,18 @@
     </row>
     <row r="32" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>48</v>
+        <v>157</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D32" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
-      <c r="E32" s="20" t="s">
-        <v>162</v>
-      </c>
+      <c r="E32" s="20"/>
       <c r="F32" s="7"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -32058,21 +32156,19 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>50</v>
+      <c r="A33" s="13" t="s">
+        <v>158</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>163</v>
+      <c r="B33" s="13" t="s">
+        <v>159</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>31</v>
+      <c r="C33" s="13" t="s">
+        <v>7</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>52</v>
+      <c r="D33" s="22" t="s">
+        <v>160</v>
       </c>
-      <c r="E33" s="20" t="s">
-        <v>164</v>
-      </c>
+      <c r="E33" s="21"/>
       <c r="F33" s="7"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -32096,19 +32192,19 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
-        <v>165</v>
+      <c r="A34" s="3" t="s">
+        <v>33</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>166</v>
+      <c r="B34" s="3" t="s">
+        <v>161</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>120</v>
+      <c r="C34" s="3" t="s">
+        <v>31</v>
       </c>
-      <c r="D34" s="18" t="s">
-        <v>167</v>
+      <c r="D34" s="5" t="s">
+        <v>46</v>
       </c>
-      <c r="E34" s="21"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="7"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -32132,15 +32228,19 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
-        <v>168</v>
+      <c r="A35" s="3" t="s">
+        <v>47</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>169</v>
+      <c r="B35" s="3" t="s">
+        <v>48</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="21"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>162</v>
+      </c>
       <c r="F35" s="7"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -32164,19 +32264,21 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
-        <v>170</v>
+      <c r="A36" s="3" t="s">
+        <v>50</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>171</v>
+      <c r="B36" s="3" t="s">
+        <v>163</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>11</v>
+      <c r="C36" s="3" t="s">
+        <v>31</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>172</v>
+      <c r="D36" s="5" t="s">
+        <v>52</v>
       </c>
-      <c r="E36" s="21"/>
+      <c r="E36" s="20" t="s">
+        <v>164</v>
+      </c>
       <c r="F36" s="7"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -32200,17 +32302,17 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
-        <v>173</v>
+      <c r="A37" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E37" s="21"/>
       <c r="F37" s="7"/>
@@ -32236,21 +32338,15 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>53</v>
+      <c r="A38" s="13" t="s">
+        <v>168</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>176</v>
+      <c r="B38" s="13" t="s">
+        <v>169</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>177</v>
-      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="21"/>
       <c r="F38" s="7"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -32274,19 +32370,19 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>56</v>
+      <c r="A39" s="16" t="s">
+        <v>170</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>178</v>
+      <c r="B39" s="13" t="s">
+        <v>171</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>31</v>
+      <c r="C39" s="13" t="s">
+        <v>11</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>58</v>
+      <c r="D39" s="18" t="s">
+        <v>172</v>
       </c>
-      <c r="E39" s="23"/>
+      <c r="E39" s="21"/>
       <c r="F39" s="7"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -32310,17 +32406,17 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>179</v>
+      <c r="A40" s="13" t="s">
+        <v>173</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E40" s="21"/>
       <c r="F40" s="7"/>
@@ -32347,18 +32443,20 @@
     </row>
     <row r="41" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
-      <c r="E41" s="21"/>
+      <c r="E41" s="23" t="s">
+        <v>177</v>
+      </c>
       <c r="F41" s="7"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -32382,19 +32480,19 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>62</v>
+      <c r="A42" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>64</v>
+      <c r="D42" s="11" t="s">
+        <v>58</v>
       </c>
-      <c r="E42" s="21"/>
+      <c r="E42" s="23"/>
       <c r="F42" s="7"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -32418,17 +32516,17 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>65</v>
+      <c r="A43" s="16" t="s">
+        <v>179</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>184</v>
+      <c r="B43" s="13" t="s">
+        <v>180</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>67</v>
+      <c r="C43" s="13" t="s">
+        <v>120</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>68</v>
+      <c r="D43" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="E43" s="21"/>
       <c r="F43" s="7"/>
@@ -32455,16 +32553,16 @@
     </row>
     <row r="44" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E44" s="21"/>
       <c r="F44" s="7"/>
@@ -32490,17 +32588,17 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
-        <v>72</v>
+      <c r="A45" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>74</v>
+      <c r="D45" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="E45" s="21"/>
       <c r="F45" s="7"/>
@@ -32526,17 +32624,17 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="8" t="s">
-        <v>75</v>
+      <c r="A46" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E46" s="21"/>
       <c r="F46" s="7"/>
@@ -32562,17 +32660,17 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
-        <v>188</v>
+      <c r="A47" s="8" t="s">
+        <v>69</v>
       </c>
-      <c r="B47" s="13" t="s">
-        <v>189</v>
+      <c r="B47" s="9" t="s">
+        <v>185</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="18" t="s">
-        <v>190</v>
+      <c r="D47" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="E47" s="21"/>
       <c r="F47" s="7"/>
@@ -32598,17 +32696,17 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="16" t="s">
-        <v>75</v>
+      <c r="A48" s="9" t="s">
+        <v>72</v>
       </c>
-      <c r="B48" s="13" t="s">
-        <v>191</v>
+      <c r="B48" s="9" t="s">
+        <v>186</v>
       </c>
-      <c r="C48" s="13" t="s">
-        <v>11</v>
+      <c r="C48" s="9" t="s">
+        <v>18</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>192</v>
+      <c r="D48" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="E48" s="21"/>
       <c r="F48" s="7"/>
@@ -32634,17 +32732,17 @@
       <c r="Z48" s="2"/>
     </row>
     <row r="49" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="16" t="s">
-        <v>193</v>
+      <c r="A49" s="8" t="s">
+        <v>75</v>
       </c>
-      <c r="B49" s="13" t="s">
-        <v>194</v>
+      <c r="B49" s="9" t="s">
+        <v>187</v>
       </c>
-      <c r="C49" s="13" t="s">
-        <v>120</v>
+      <c r="C49" s="9" t="s">
+        <v>11</v>
       </c>
-      <c r="D49" s="18" t="s">
-        <v>195</v>
+      <c r="D49" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="E49" s="21"/>
       <c r="F49" s="7"/>
@@ -32670,14 +32768,18 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
-        <v>196</v>
+      <c r="A50" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
+      <c r="C50" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>190</v>
+      </c>
       <c r="E50" s="21"/>
       <c r="F50" s="7"/>
       <c r="G50" s="2"/>
@@ -32702,14 +32804,18 @@
       <c r="Z50" s="2"/>
     </row>
     <row r="51" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
-        <v>198</v>
+      <c r="A51" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
+      <c r="C51" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>192</v>
+      </c>
       <c r="E51" s="21"/>
       <c r="F51" s="7"/>
       <c r="G51" s="2"/>
@@ -32734,17 +32840,17 @@
       <c r="Z51" s="2"/>
     </row>
     <row r="52" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13" t="s">
-        <v>200</v>
+      <c r="A52" s="16" t="s">
+        <v>193</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E52" s="21"/>
       <c r="F52" s="7"/>
@@ -32770,18 +32876,14 @@
       <c r="Z52" s="2"/>
     </row>
     <row r="53" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="9" t="s">
-        <v>78</v>
+      <c r="A53" s="13" t="s">
+        <v>196</v>
       </c>
-      <c r="B53" s="9" t="s">
-        <v>203</v>
+      <c r="B53" s="13" t="s">
+        <v>197</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>80</v>
-      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
       <c r="E53" s="21"/>
       <c r="F53" s="7"/>
       <c r="G53" s="2"/>
@@ -32807,17 +32909,13 @@
     </row>
     <row r="54" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
-        <v>78</v>
+        <v>198</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
-      <c r="C54" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>205</v>
-      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
       <c r="E54" s="21"/>
       <c r="F54" s="7"/>
       <c r="G54" s="2"/>
@@ -32843,16 +32941,16 @@
     </row>
     <row r="55" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
-        <v>78</v>
+        <v>200</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E55" s="21"/>
       <c r="F55" s="7"/>
@@ -32878,17 +32976,17 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>208</v>
+      <c r="B56" s="9" t="s">
+        <v>203</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="18" t="s">
-        <v>209</v>
+      <c r="D56" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="E56" s="21"/>
       <c r="F56" s="7"/>
@@ -32918,13 +33016,13 @@
         <v>78</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E57" s="21"/>
       <c r="F57" s="7"/>
@@ -32954,13 +33052,13 @@
         <v>78</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E58" s="21"/>
       <c r="F58" s="7"/>
@@ -32987,16 +33085,16 @@
     </row>
     <row r="59" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E59" s="21"/>
       <c r="F59" s="7"/>
@@ -33026,13 +33124,13 @@
         <v>78</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="E60" s="21"/>
       <c r="F60" s="7"/>
@@ -33062,13 +33160,13 @@
         <v>78</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E61" s="21"/>
       <c r="F61" s="7"/>
@@ -33095,13 +33193,17 @@
     </row>
     <row r="62" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
+      <c r="C62" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>216</v>
+      </c>
       <c r="E62" s="21"/>
       <c r="F62" s="7"/>
       <c r="G62" s="2"/>
@@ -33127,13 +33229,17 @@
     </row>
     <row r="63" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>223</v>
+        <v>78</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
+      <c r="C63" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>218</v>
+      </c>
       <c r="E63" s="21"/>
       <c r="F63" s="7"/>
       <c r="G63" s="2"/>
@@ -33162,13 +33268,13 @@
         <v>78</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E64" s="21"/>
       <c r="F64" s="7"/>
@@ -33195,17 +33301,13 @@
     </row>
     <row r="65" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
-      <c r="C65" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>229</v>
-      </c>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
       <c r="E65" s="21"/>
       <c r="F65" s="7"/>
       <c r="G65" s="2"/>
@@ -33230,18 +33332,14 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="9" t="s">
-        <v>81</v>
+      <c r="A66" s="13" t="s">
+        <v>223</v>
       </c>
-      <c r="B66" s="9" t="s">
-        <v>230</v>
+      <c r="B66" s="13" t="s">
+        <v>224</v>
       </c>
-      <c r="C66" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>83</v>
-      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
       <c r="E66" s="21"/>
       <c r="F66" s="7"/>
       <c r="G66" s="2"/>
@@ -33267,13 +33365,17 @@
     </row>
     <row r="67" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>231</v>
+        <v>78</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
+      <c r="C67" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>226</v>
+      </c>
       <c r="E67" s="21"/>
       <c r="F67" s="7"/>
       <c r="G67" s="2"/>
@@ -33298,20 +33400,20 @@
       <c r="Z67" s="2"/>
     </row>
     <row r="68" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="9" t="s">
-        <v>84</v>
+      <c r="A68" s="13" t="s">
+        <v>227</v>
       </c>
-      <c r="B68" s="9" t="s">
-        <v>233</v>
+      <c r="B68" s="13" t="s">
+        <v>228</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>7</v>
+      <c r="C68" s="13" t="s">
+        <v>31</v>
       </c>
-      <c r="D68" s="11" t="s">
-        <v>86</v>
+      <c r="D68" s="18" t="s">
+        <v>229</v>
       </c>
       <c r="E68" s="21"/>
-      <c r="F68" s="2"/>
+      <c r="F68" s="7"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -33334,12 +33436,20 @@
       <c r="Z68" s="2"/>
     </row>
     <row r="69" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="13"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
+      <c r="A69" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="E69" s="21"/>
-      <c r="F69" s="2"/>
+      <c r="F69" s="7"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -33362,12 +33472,16 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="13"/>
-      <c r="B70" s="13"/>
+      <c r="A70" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>232</v>
+      </c>
       <c r="C70" s="13"/>
       <c r="D70" s="13"/>
       <c r="E70" s="21"/>
-      <c r="F70" s="2"/>
+      <c r="F70" s="7"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -33390,10 +33504,18 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
+      <c r="A71" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="E71" s="21"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -33418,11 +33540,11 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="24"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="21"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
@@ -33446,11 +33568,11 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="24"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="21"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
@@ -33474,11 +33596,11 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="24"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="21"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
@@ -59429,62 +59551,149 @@
       <c r="Y1000" s="2"/>
       <c r="Z1000" s="2"/>
     </row>
+    <row r="1001" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1001" s="14"/>
+      <c r="B1001" s="14"/>
+      <c r="C1001" s="14"/>
+      <c r="D1001" s="14"/>
+      <c r="E1001" s="24"/>
+      <c r="F1001" s="2"/>
+      <c r="G1001" s="2"/>
+      <c r="H1001" s="2"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="2"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="2"/>
+      <c r="M1001" s="2"/>
+      <c r="N1001" s="2"/>
+      <c r="O1001" s="2"/>
+      <c r="P1001" s="2"/>
+      <c r="Q1001" s="2"/>
+      <c r="R1001" s="2"/>
+      <c r="S1001" s="2"/>
+      <c r="T1001" s="2"/>
+      <c r="U1001" s="2"/>
+      <c r="V1001" s="2"/>
+      <c r="W1001" s="2"/>
+      <c r="X1001" s="2"/>
+      <c r="Y1001" s="2"/>
+      <c r="Z1001" s="2"/>
+    </row>
+    <row r="1002" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1002" s="14"/>
+      <c r="B1002" s="14"/>
+      <c r="C1002" s="14"/>
+      <c r="D1002" s="14"/>
+      <c r="E1002" s="24"/>
+      <c r="F1002" s="2"/>
+      <c r="G1002" s="2"/>
+      <c r="H1002" s="2"/>
+      <c r="I1002" s="2"/>
+      <c r="J1002" s="2"/>
+      <c r="K1002" s="2"/>
+      <c r="L1002" s="2"/>
+      <c r="M1002" s="2"/>
+      <c r="N1002" s="2"/>
+      <c r="O1002" s="2"/>
+      <c r="P1002" s="2"/>
+      <c r="Q1002" s="2"/>
+      <c r="R1002" s="2"/>
+      <c r="S1002" s="2"/>
+      <c r="T1002" s="2"/>
+      <c r="U1002" s="2"/>
+      <c r="V1002" s="2"/>
+      <c r="W1002" s="2"/>
+      <c r="X1002" s="2"/>
+      <c r="Y1002" s="2"/>
+      <c r="Z1002" s="2"/>
+    </row>
+    <row r="1003" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1003" s="14"/>
+      <c r="B1003" s="14"/>
+      <c r="C1003" s="14"/>
+      <c r="D1003" s="14"/>
+      <c r="E1003" s="24"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="2"/>
+      <c r="H1003" s="2"/>
+      <c r="I1003" s="2"/>
+      <c r="J1003" s="2"/>
+      <c r="K1003" s="2"/>
+      <c r="L1003" s="2"/>
+      <c r="M1003" s="2"/>
+      <c r="N1003" s="2"/>
+      <c r="O1003" s="2"/>
+      <c r="P1003" s="2"/>
+      <c r="Q1003" s="2"/>
+      <c r="R1003" s="2"/>
+      <c r="S1003" s="2"/>
+      <c r="T1003" s="2"/>
+      <c r="U1003" s="2"/>
+      <c r="V1003" s="2"/>
+      <c r="W1003" s="2"/>
+      <c r="X1003" s="2"/>
+      <c r="Y1003" s="2"/>
+      <c r="Z1003" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="D12" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="E12" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="E14" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="D15" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="D17" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="D19" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="D20" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="D21" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="D22" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="D23" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="D24" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="D25" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="D26" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="D28" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="D29" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="D30" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="D31" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="D32" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="D33" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="D34" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="D36" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="D37" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="D38" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="D39" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="D40" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="D41" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="D42" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="D43" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="D44" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="D45" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="D46" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="D47" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="D49" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="D52" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="D53" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="D54" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="D55" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="D56" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="D57" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="D58" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="D59" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="D60" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="D61" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="D64" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="D65" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="D66" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="D68" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D11" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D12" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D14" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D15" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E15" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="D16" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E17" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="D18" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="D20" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="D22" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="D23" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="D24" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="D25" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="D26" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="D27" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="D28" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="D29" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="D31" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="D32" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="D33" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="D34" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="D35" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="D36" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="D37" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="D39" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="D40" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="D41" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="D42" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="D43" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="D44" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="D45" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="D46" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="D47" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="D48" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="D49" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="D50" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="D52" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="D55" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="D56" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="D57" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="D58" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="D59" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="D60" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="D61" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="D62" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="D63" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="D64" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="D67" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="D68" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="D69" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="D71" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="D8" r:id="rId55" xr:uid="{3F825C91-7801-6A44-9B78-953241B1155A}"/>
+    <hyperlink ref="D7" r:id="rId56" xr:uid="{9F4BCCFA-A0E3-B84E-9F7D-67A6B790FBE8}"/>
+    <hyperlink ref="D6" r:id="rId57" xr:uid="{0C701F3B-8F0C-4F4C-B313-9C68EF731B3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>